<commit_message>
Convertation to the sheet
</commit_message>
<xml_diff>
--- a/data/turm/ELT-1A.xlsx
+++ b/data/turm/ELT-1A.xlsx
@@ -441,34 +441,34 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>segunda</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>terça</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>quarta</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>quinta</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>sexta</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -500,7 +500,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7:50</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -525,14 +525,14 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Desenho Técnico</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>8:40</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -564,7 +564,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>9:30</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -589,14 +589,14 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>EAP</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10:40</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -611,12 +611,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Circuitos Elétricos 2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Circuitos Elétricos 2</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -628,7 +628,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>11:30</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -653,14 +653,14 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAP</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -692,7 +692,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13:50</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14:40</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -734,7 +734,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>EAP</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -756,7 +756,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15:30</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -820,7 +820,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>17:30</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -840,12 +840,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Desenho Técnico</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>EAP</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix error of turm classes being only one
</commit_message>
<xml_diff>
--- a/data/turm/ELT-1A.xlsx
+++ b/data/turm/ELT-1A.xlsx
@@ -525,7 +525,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Desenho Técnico</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Desenho Técnico</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -606,12 +606,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Desenho Técnico</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Circuitos Elétricos 2</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -653,7 +653,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>EAP</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -845,7 +845,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>EAP</t>
+          <t>-</t>
         </is>
       </c>
     </row>

</xml_diff>